<commit_message>
[MOD] Tabelle strategia 3 complete
</commit_message>
<xml_diff>
--- a/Esercitazione3/Tabelle_Strategia3.xlsx
+++ b/Esercitazione3/Tabelle_Strategia3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\OneDrive\Desktop\Universita\Informatica\Magistrale\Anno_2\Metodi_Numerici\MNI_Esercizi\Esercitazione3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC857CFA-DD71-46D7-AFE4-612ABAFDB6B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B495AB6-0C2B-4B47-9BC4-A6A5B0CD15F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12600" yWindow="1785" windowWidth="18420" windowHeight="14595" xr2:uid="{BFBD3147-2A7D-4227-A28A-85E78CD98EEF}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{BFBD3147-2A7D-4227-A28A-85E78CD98EEF}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -69,9 +69,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="#,##0.000"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -179,7 +180,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -199,6 +200,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -826,19 +828,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1.790083632019116</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>2.2172808132147397</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1.8718340982491926</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1.9307605232265639</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1.7406154322439535</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -911,19 +913,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2.2888787045523986</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>3.8002940055534387</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>3.3147208885811899</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>3.3017633542087133</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>2.4931738980515461</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -996,19 +998,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2.3984312469985589</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>3.5997937080969571</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>3.9702197465433637</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>4.3579370712088954</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>3.5699008521213353</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1487,19 +1489,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.89504181600955801</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1.1086404066073698</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.93591704912459628</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.96538026161328194</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.87030771612197677</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1572,19 +1574,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.57221967613809965</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.95007350138835966</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.82868022214529746</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.82544083855217831</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.62329347451288653</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1657,19 +1659,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.29980390587481986</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.44997421351211964</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.49627746831792047</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.54474213390111192</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.44623760651516692</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3556,8 +3558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3725E956-6166-4304-922D-C2C0C8EF654E}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3675,14 +3677,16 @@
       <c r="B11" s="4">
         <v>1000</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="3" t="e">
+      <c r="C11" s="2">
+        <v>0.83699999999999997</v>
+      </c>
+      <c r="D11" s="3">
         <f>C3/C11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E11" s="3" t="e">
+        <v>1.790083632019116</v>
+      </c>
+      <c r="E11" s="3">
         <f>D11/2</f>
-        <v>#DIV/0!</v>
+        <v>0.89504181600955801</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -3692,14 +3696,16 @@
       <c r="B12" s="4">
         <v>2000</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="8" t="e">
+      <c r="C12" s="2">
+        <v>3.1480000000000001</v>
+      </c>
+      <c r="D12" s="8">
         <f>C4/C12</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E12" s="3" t="e">
+        <v>2.2172808132147397</v>
+      </c>
+      <c r="E12" s="3">
         <f>D12/2</f>
-        <v>#DIV/0!</v>
+        <v>1.1086404066073698</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -3709,14 +3715,16 @@
       <c r="B13" s="4">
         <v>4000</v>
       </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="3" t="e">
+      <c r="C13" s="2">
+        <v>11.766</v>
+      </c>
+      <c r="D13" s="3">
         <f>C5/C13</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E13" s="3" t="e">
+        <v>1.8718340982491926</v>
+      </c>
+      <c r="E13" s="3">
         <f>D13/2</f>
-        <v>#DIV/0!</v>
+        <v>0.93591704912459628</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -3726,14 +3734,16 @@
       <c r="B14" s="4">
         <v>8000</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="8" t="e">
+      <c r="C14" s="2">
+        <v>47.704000000000001</v>
+      </c>
+      <c r="D14" s="8">
         <f>C6/C14</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E14" s="3" t="e">
+        <v>1.9307605232265639</v>
+      </c>
+      <c r="E14" s="3">
         <f>D14/2</f>
-        <v>#DIV/0!</v>
+        <v>0.96538026161328194</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -3743,14 +3753,16 @@
       <c r="B15" s="4">
         <v>16000</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="3" t="e">
+      <c r="C15" s="2">
+        <v>198.97559999999999</v>
+      </c>
+      <c r="D15" s="3">
         <f>C7/C15</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E15" s="3" t="e">
+        <v>1.7406154322439535</v>
+      </c>
+      <c r="E15" s="3">
         <f>D15/2</f>
-        <v>#DIV/0!</v>
+        <v>0.87030771612197677</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -3791,14 +3803,16 @@
       <c r="B19" s="4">
         <v>1000</v>
       </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="3" t="e">
+      <c r="C19" s="2">
+        <v>0.65459999999999996</v>
+      </c>
+      <c r="D19" s="3">
         <f>C3/C19</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E19" s="3" t="e">
+        <v>2.2888787045523986</v>
+      </c>
+      <c r="E19" s="3">
         <f>D19/4</f>
-        <v>#DIV/0!</v>
+        <v>0.57221967613809965</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -3808,14 +3822,16 @@
       <c r="B20" s="4">
         <v>2000</v>
       </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="3" t="e">
+      <c r="C20" s="2">
+        <v>1.8367</v>
+      </c>
+      <c r="D20" s="3">
         <f>C4/C20</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E20" s="3" t="e">
+        <v>3.8002940055534387</v>
+      </c>
+      <c r="E20" s="3">
         <f>D20/4</f>
-        <v>#DIV/0!</v>
+        <v>0.95007350138835966</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -3825,14 +3841,16 @@
       <c r="B21" s="4">
         <v>4000</v>
       </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="3" t="e">
+      <c r="C21" s="2">
+        <v>6.6443000000000003</v>
+      </c>
+      <c r="D21" s="3">
         <f>C5/C21</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E21" s="3" t="e">
+        <v>3.3147208885811899</v>
+      </c>
+      <c r="E21" s="3">
         <f>D21/4</f>
-        <v>#DIV/0!</v>
+        <v>0.82868022214529746</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -3842,14 +3860,16 @@
       <c r="B22" s="4">
         <v>8000</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="3" t="e">
+      <c r="C22" s="2">
+        <v>27.895700000000001</v>
+      </c>
+      <c r="D22" s="3">
         <f>C6/C22</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E22" s="3" t="e">
+        <v>3.3017633542087133</v>
+      </c>
+      <c r="E22" s="3">
         <f>D22/4</f>
-        <v>#DIV/0!</v>
+        <v>0.82544083855217831</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -3859,14 +3879,16 @@
       <c r="B23" s="4">
         <v>16000</v>
       </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="8" t="e">
+      <c r="C23" s="2">
+        <v>138.9153</v>
+      </c>
+      <c r="D23" s="8">
         <f>C7/C23</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E23" s="3" t="e">
+        <v>2.4931738980515461</v>
+      </c>
+      <c r="E23" s="3">
         <f>D23/4</f>
-        <v>#DIV/0!</v>
+        <v>0.62329347451288653</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -3913,14 +3935,16 @@
       <c r="B28" s="4">
         <v>1000</v>
       </c>
-      <c r="C28" s="2"/>
-      <c r="D28" s="3" t="e">
+      <c r="C28" s="2">
+        <v>0.62470000000000003</v>
+      </c>
+      <c r="D28" s="3">
         <f>C3/C28</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E28" s="3" t="e">
+        <v>2.3984312469985589</v>
+      </c>
+      <c r="E28" s="3">
         <f>D28/8</f>
-        <v>#DIV/0!</v>
+        <v>0.29980390587481986</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -3930,14 +3954,16 @@
       <c r="B29" s="4">
         <v>2000</v>
       </c>
-      <c r="C29" s="2"/>
-      <c r="D29" s="3" t="e">
+      <c r="C29" s="2">
+        <v>1.9390000000000001</v>
+      </c>
+      <c r="D29" s="3">
         <f>C4/C29</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E29" s="3" t="e">
+        <v>3.5997937080969571</v>
+      </c>
+      <c r="E29" s="3">
         <f>D29/8</f>
-        <v>#DIV/0!</v>
+        <v>0.44997421351211964</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -3947,14 +3973,16 @@
       <c r="B30" s="4">
         <v>4000</v>
       </c>
-      <c r="C30" s="2"/>
-      <c r="D30" s="3" t="e">
+      <c r="C30" s="2">
+        <v>5.5472999999999999</v>
+      </c>
+      <c r="D30" s="3">
         <f>C5/C30</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E30" s="3" t="e">
+        <v>3.9702197465433637</v>
+      </c>
+      <c r="E30" s="3">
         <f>D30/8</f>
-        <v>#DIV/0!</v>
+        <v>0.49627746831792047</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -3964,14 +3992,16 @@
       <c r="B31" s="4">
         <v>8000</v>
       </c>
-      <c r="C31" s="7"/>
-      <c r="D31" s="3" t="e">
+      <c r="C31" s="13">
+        <v>21.135000000000002</v>
+      </c>
+      <c r="D31" s="3">
         <f>C6/C31</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E31" s="3" t="e">
+        <v>4.3579370712088954</v>
+      </c>
+      <c r="E31" s="3">
         <f>D31/8</f>
-        <v>#DIV/0!</v>
+        <v>0.54474213390111192</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -3981,14 +4011,16 @@
       <c r="B32" s="4">
         <v>16000</v>
       </c>
-      <c r="C32" s="7"/>
-      <c r="D32" s="3" t="e">
+      <c r="C32" s="7">
+        <v>97.0167</v>
+      </c>
+      <c r="D32" s="3">
         <f>C7/C32</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E32" s="3" t="e">
+        <v>3.5699008521213353</v>
+      </c>
+      <c r="E32" s="3">
         <f>D32/8</f>
-        <v>#DIV/0!</v>
+        <v>0.44623760651516692</v>
       </c>
     </row>
   </sheetData>

</xml_diff>